<commit_message>
uporządkowanie folderu z obrazkami, poprawka w skrypcie sql
</commit_message>
<xml_diff>
--- a/planszo_kreator.xlsx
+++ b/planszo_kreator.xlsx
@@ -377,84 +377,12 @@
     <cellStyle name="Result" xfId="6"/>
     <cellStyle name="Result2" xfId="7"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF333333"/>
           <bgColor rgb="FF333333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF333333"/>
-          <bgColor rgb="FF333333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF333333"/>
-          <bgColor rgb="FF333333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF333333"/>
-          <bgColor rgb="FF333333"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -597,16 +525,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF999999"/>
-          <bgColor rgb="FF999999"/>
+          <fgColor rgb="FF333333"/>
+          <bgColor rgb="FF333333"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF333333"/>
-          <bgColor rgb="FF333333"/>
+          <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF999999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1722,12 +1650,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2530,12 +2458,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="13" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3669,12 +3597,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A27:J36">
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>A16&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:J25">
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3957,8 +3885,8 @@
         <v>1</v>
       </c>
       <c r="L5" t="str">
-        <f>"INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES ("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(A5)-4&amp;",0,"&amp;A5&amp;","&amp;A16&amp;","&amp;A27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(B5)-4&amp;",1,"&amp;B5&amp;","&amp;B16&amp;","&amp;B27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(C5)-4&amp;",2,"&amp;C5&amp;","&amp;C16&amp;","&amp;C27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(D5)-4&amp;",3,"&amp;D5&amp;","&amp;D16&amp;","&amp;D27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(E5)-4&amp;",4,"&amp;E5&amp;","&amp;E16&amp;","&amp;E27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(F5)-4&amp;",5,"&amp;F5&amp;","&amp;F16&amp;","&amp;F27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(G5)-4&amp;",6,"&amp;G5&amp;","&amp;G16&amp;","&amp;G27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(H5)-4&amp;",7,"&amp;H5&amp;","&amp;H16&amp;","&amp;H27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(I5)-4&amp;",8,"&amp;I5&amp;","&amp;I16&amp;","&amp;I27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(J5)-4&amp;",9,"&amp;J5&amp;","&amp;J16&amp;","&amp;J27&amp;");"</f>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,1,0,1,104,0),(0,0,1,1,1,102,0),(0,0,1,2,1,101,0),(0,0,1,3,1,102,0),(0,0,1,4,1,101,0),(0,0,1,5,1,104,0),(0,0,1,6,1,102,0),(0,0,1,7,1,101,0),(0,0,1,8,1,102,0),(0,0,1,9,1,100,0);</v>
+        <f>"INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES ("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(A5)-5&amp;",0,"&amp;A5&amp;","&amp;A16&amp;","&amp;A27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(B5)-5&amp;",1,"&amp;B5&amp;","&amp;B16&amp;","&amp;B27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(C5)-5&amp;",2,"&amp;C5&amp;","&amp;C16&amp;","&amp;C27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(D5)-5&amp;",3,"&amp;D5&amp;","&amp;D16&amp;","&amp;D27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(E5)-5&amp;",4,"&amp;E5&amp;","&amp;E16&amp;","&amp;E27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(F5)-5&amp;",5,"&amp;F5&amp;","&amp;F16&amp;","&amp;F27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(G5)-5&amp;",6,"&amp;G5&amp;","&amp;G16&amp;","&amp;G27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(H5)-5&amp;",7,"&amp;H5&amp;","&amp;H16&amp;","&amp;H27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(I5)-5&amp;",8,"&amp;I5&amp;","&amp;I16&amp;","&amp;I27&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(J5)-5&amp;",9,"&amp;J5&amp;","&amp;J16&amp;","&amp;J27&amp;");"</f>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,0,0,1,104,0),(0,0,0,1,1,102,0),(0,0,0,2,1,101,0),(0,0,0,3,1,102,0),(0,0,0,4,1,101,0),(0,0,0,5,1,104,0),(0,0,0,6,1,102,0),(0,0,0,7,1,101,0),(0,0,0,8,1,102,0),(0,0,0,9,1,100,0);</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3993,8 +3921,8 @@
         <v>1</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" ref="L6:L14" si="0">"INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES ("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(A6)-4&amp;",0,"&amp;A6&amp;","&amp;A17&amp;","&amp;A28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(B6)-4&amp;",1,"&amp;B6&amp;","&amp;B17&amp;","&amp;B28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(C6)-4&amp;",2,"&amp;C6&amp;","&amp;C17&amp;","&amp;C28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(D6)-4&amp;",3,"&amp;D6&amp;","&amp;D17&amp;","&amp;D28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(E6)-4&amp;",4,"&amp;E6&amp;","&amp;E17&amp;","&amp;E28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(F6)-4&amp;",5,"&amp;F6&amp;","&amp;F17&amp;","&amp;F28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(G6)-4&amp;",6,"&amp;G6&amp;","&amp;G17&amp;","&amp;G28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(H6)-4&amp;",7,"&amp;H6&amp;","&amp;H17&amp;","&amp;H28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(I6)-4&amp;",8,"&amp;I6&amp;","&amp;I17&amp;","&amp;I28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(J6)-4&amp;",9,"&amp;J6&amp;","&amp;J17&amp;","&amp;J28&amp;");"</f>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,2,0,1,103,0),(0,0,2,1,1,103,0),(0,0,2,2,1,100,0),(0,0,2,3,1,101,0),(0,0,2,4,1,106,0),(0,0,2,5,1,107,0),(0,0,2,6,1,103,0),(0,0,2,7,1,101,0),(0,0,2,8,1,102,0),(0,0,2,9,1,0,0);</v>
+        <f t="shared" ref="L6:L14" si="0">"INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES ("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(A6)-5&amp;",0,"&amp;A6&amp;","&amp;A17&amp;","&amp;A28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(B6)-5&amp;",1,"&amp;B6&amp;","&amp;B17&amp;","&amp;B28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(C6)-5&amp;",2,"&amp;C6&amp;","&amp;C17&amp;","&amp;C28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(D6)-5&amp;",3,"&amp;D6&amp;","&amp;D17&amp;","&amp;D28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(E6)-5&amp;",4,"&amp;E6&amp;","&amp;E17&amp;","&amp;E28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(F6)-5&amp;",5,"&amp;F6&amp;","&amp;F17&amp;","&amp;F28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(G6)-5&amp;",6,"&amp;G6&amp;","&amp;G17&amp;","&amp;G28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(H6)-5&amp;",7,"&amp;H6&amp;","&amp;H17&amp;","&amp;H28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(I6)-5&amp;",8,"&amp;I6&amp;","&amp;I17&amp;","&amp;I28&amp;"),("&amp;$L$3&amp;","&amp;$M$3&amp;","&amp;ROW(J6)-5&amp;",9,"&amp;J6&amp;","&amp;J17&amp;","&amp;J28&amp;");"</f>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,1,0,1,103,0),(0,0,1,1,1,103,0),(0,0,1,2,1,100,0),(0,0,1,3,1,101,0),(0,0,1,4,1,106,0),(0,0,1,5,1,107,0),(0,0,1,6,1,103,0),(0,0,1,7,1,101,0),(0,0,1,8,1,102,0),(0,0,1,9,1,0,0);</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4030,7 +3958,7 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,3,0,1,102,0),(0,0,3,1,1,101,0),(0,0,3,2,1,104,0),(0,0,3,3,1,0,0),(0,0,3,4,1,0,0),(0,0,3,5,1,0,0),(0,0,3,6,1,103,0),(0,0,3,7,1,104,0),(0,0,3,8,1,0,0),(0,0,3,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,2,0,1,102,0),(0,0,2,1,1,101,0),(0,0,2,2,1,104,0),(0,0,2,3,1,0,0),(0,0,2,4,1,0,0),(0,0,2,5,1,0,0),(0,0,2,6,1,103,0),(0,0,2,7,1,104,0),(0,0,2,8,1,0,0),(0,0,2,9,1,0,0);</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4066,7 +3994,7 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,4,0,1,103,0),(0,0,4,1,1,102,0),(0,0,4,2,1,0,0),(0,0,4,3,1,0,0),(0,0,4,4,1,0,0),(0,0,4,5,1,0,0),(0,0,4,6,1,0,1),(0,0,4,7,1,103,0),(0,0,4,8,1,0,0),(0,0,4,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,3,0,1,103,0),(0,0,3,1,1,102,0),(0,0,3,2,1,0,0),(0,0,3,3,1,0,0),(0,0,3,4,1,0,0),(0,0,3,5,1,0,0),(0,0,3,6,1,0,1),(0,0,3,7,1,103,0),(0,0,3,8,1,0,0),(0,0,3,9,1,0,0);</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4105,7 +4033,7 @@
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,5,0,1,101,0),(0,0,5,1,1,100,0),(0,0,5,2,1,0,0),(0,0,5,3,1,0,0),(0,0,5,4,1,105,0),(0,0,5,5,1,0,0),(0,0,5,6,1,0,0),(0,0,5,7,1,0,0),(0,0,5,8,1,0,0),(0,0,5,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,4,0,1,101,0),(0,0,4,1,1,100,0),(0,0,4,2,1,0,0),(0,0,4,3,1,0,0),(0,0,4,4,1,105,0),(0,0,4,5,1,0,0),(0,0,4,6,1,0,0),(0,0,4,7,1,0,0),(0,0,4,8,1,0,0),(0,0,4,9,1,0,0);</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4141,7 +4069,7 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,6,0,1,100,0),(0,0,6,1,1,100,0),(0,0,6,2,1,102,0),(0,0,6,3,1,0,0),(0,0,6,4,1,0,0),(0,0,6,5,1,0,0),(0,0,6,6,1,0,0),(0,0,6,7,1,0,0),(0,0,6,8,1,0,0),(0,0,6,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,5,0,1,100,0),(0,0,5,1,1,100,0),(0,0,5,2,1,102,0),(0,0,5,3,1,0,0),(0,0,5,4,1,0,0),(0,0,5,5,1,0,0),(0,0,5,6,1,0,0),(0,0,5,7,1,0,0),(0,0,5,8,1,0,0),(0,0,5,9,1,0,0);</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4177,7 +4105,7 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,7,0,1,100,0),(0,0,7,1,1,100,0),(0,0,7,2,1,0,1),(0,0,7,3,1,0,0),(0,0,7,4,1,0,0),(0,0,7,5,1,0,0),(0,0,7,6,1,0,0),(0,0,7,7,1,0,0),(0,0,7,8,1,0,0),(0,0,7,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,6,0,1,100,0),(0,0,6,1,1,100,0),(0,0,6,2,1,0,1),(0,0,6,3,1,0,0),(0,0,6,4,1,0,0),(0,0,6,5,1,0,0),(0,0,6,6,1,0,0),(0,0,6,7,1,0,0),(0,0,6,8,1,0,0),(0,0,6,9,1,0,0);</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4213,7 +4141,7 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,8,0,1,101,0),(0,0,8,1,1,101,0),(0,0,8,2,1,104,0),(0,0,8,3,1,0,0),(0,0,8,4,1,0,1),(0,0,8,5,1,103,0),(0,0,8,6,1,102,0),(0,0,8,7,1,0,0),(0,0,8,8,1,0,0),(0,0,8,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,7,0,1,101,0),(0,0,7,1,1,101,0),(0,0,7,2,1,104,0),(0,0,7,3,1,0,0),(0,0,7,4,1,0,1),(0,0,7,5,1,103,0),(0,0,7,6,1,102,0),(0,0,7,7,1,0,0),(0,0,7,8,1,0,0),(0,0,7,9,1,0,0);</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4249,7 +4177,7 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,9,0,1,101,0),(0,0,9,1,1,103,0),(0,0,9,2,1,0,0),(0,0,9,3,1,0,0),(0,0,9,4,1,0,0),(0,0,9,5,1,0,0),(0,0,9,6,1,0,0),(0,0,9,7,1,0,0),(0,0,9,8,1,0,0),(0,0,9,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,8,0,1,101,0),(0,0,8,1,1,103,0),(0,0,8,2,1,0,0),(0,0,8,3,1,0,0),(0,0,8,4,1,0,0),(0,0,8,5,1,0,0),(0,0,8,6,1,0,0),(0,0,8,7,1,0,0),(0,0,8,8,1,0,0),(0,0,8,9,1,0,0);</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4285,7 +4213,7 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,10,0,1,103,0),(0,0,10,1,1,0,0),(0,0,10,2,1,0,0),(0,0,10,3,1,0,0),(0,0,10,4,1,0,0),(0,0,10,5,1,0,0),(0,0,10,6,1,0,0),(0,0,10,7,1,0,0),(0,0,10,8,1,0,0),(0,0,10,9,1,0,0);</v>
+        <v>INSERT INTO pola(planszax, planszay, x , y, podloze, rodzaj, stwor) VALUES (0,0,9,0,1,103,0),(0,0,9,1,1,0,0),(0,0,9,2,1,0,0),(0,0,9,3,1,0,0),(0,0,9,4,1,0,0),(0,0,9,5,1,0,0),(0,0,9,6,1,0,0),(0,0,9,7,1,0,0),(0,0,9,8,1,0,0),(0,0,9,9,1,0,0);</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5007,12 +4935,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A27:J36">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
       <formula>A16&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:J25">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5816,12 +5744,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="27" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6622,12 +6550,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="25" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7428,12 +7356,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="23" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8234,12 +8162,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9049,12 +8977,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="19" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9855,12 +9783,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10661,12 +10589,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:J24">
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>A1&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>